<commit_message>
read Sheet by Name instead of Index
</commit_message>
<xml_diff>
--- a/06112023/src/test/resources/testdata/excel/TestData.xlsx
+++ b/06112023/src/test/resources/testdata/excel/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\ApachePOI_19Sep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neeraj Aggarwal\git\Selenium-WebDriver-With-Java-By-Neeraj-Aggarwal\06112023\src\test\resources\testdata\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435EAE45-CB9B-4396-A52B-A5ED696E8BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4715C1CE-A5BC-402C-8FEE-4DB800E2F3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="read" sheetId="1" r:id="rId1"/>
@@ -378,9 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -479,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE26FDE-6325-4D5A-9F86-79A3807D54A4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated The Sample Code to read and write excel file using Apache POI
</commit_message>
<xml_diff>
--- a/06112023/src/test/resources/testdata/excel/TestData.xlsx
+++ b/06112023/src/test/resources/testdata/excel/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neeraj Aggarwal\git\Selenium-WebDriver-With-Java-By-Neeraj-Aggarwal\06112023\src\test\resources\testdata\excel\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -59,12 +59,25 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>Updated using Apache POI Library</t>
+  </si>
+  <si>
+    <t>Updated using Apache POI Library at:Sun Oct 13 11:50:09 IST 2024</t>
+  </si>
+  <si>
+    <t>Updated using Apache POI Library on Sun Oct 13 11:51:18 IST 2024</t>
+  </si>
+  <si>
+    <t>Updated using Apache POI Library on Sun Oct 13 11:52:11 IST 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,89 +395,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.88671875"/>
+    <col min="2" max="2" customWidth="true" width="11.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.33203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>10</v>
       </c>
     </row>
@@ -475,7 +488,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE26FDE-6325-4D5A-9F86-79A3807D54A4}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -483,87 +496,117 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="C4" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>4</v>
       </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>5</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="C7" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="C9" t="s" s="0">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>10</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>